<commit_message>
Oops, forgot the nozzle
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3d printing\stormwalker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5E74A8-8051-4103-BF88-D3EB5E0E561C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0E3361-B23B-49E7-A0ED-7095095644A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9936" yWindow="5268" windowWidth="27276" windowHeight="22044" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="27276" windowHeight="22044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Body" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="303">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1402,6 +1402,14 @@
   </si>
   <si>
     <t>Fly-C8 doesn't support the addon WiFi module if you don't use the bloat filled system image. Flawless design.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bimetal Nozzle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bimetal Volcano Nozzle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1861,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E69"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2443,6 +2451,17 @@
         <v>216</v>
       </c>
       <c r="D43" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D44" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2751,7 +2770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6375C457-B0C0-4589-A3C9-93DBFBDBB730}">
   <dimension ref="A2:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Use SMT thermistor on the bed which is more reliable and cheaper
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3d printing\stormwalker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0E3361-B23B-49E7-A0ED-7095095644A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE9DCC0-536A-4F6D-98A1-2A818E25165A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="27276" windowHeight="22044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="27276" windowHeight="22044" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Body" sheetId="1" r:id="rId1"/>
@@ -339,10 +339,6 @@
   </si>
   <si>
     <t>Thermister</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cartridge</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -587,10 +583,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UL 1332 FEP insulated wire</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Wire</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -631,14 +623,6 @@
   </si>
   <si>
     <t>2m</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Non-Split Braided Sleeving</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -766,10 +750,6 @@
   </si>
   <si>
     <t>For wiring heaters and fans.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10m</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1036,10 +1016,6 @@
   </si>
   <si>
     <t>M1.6x2.5x5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Generic 3950</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1361,10 +1337,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>For bed. Alternatively cut up a high wattage USB cable.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GND</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1410,6 +1382,34 @@
   </si>
   <si>
     <t>Bimetal Volcano Nozzle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Surface Mounted 0805 Size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Generic 3950 100K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insulated wire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Silicone wire 4 Strand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>230mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For bed heater and thermistor.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1869,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52:E53"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1983,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2024,7 +2024,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
@@ -2038,7 +2038,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="7">
         <v>2</v>
@@ -2084,7 +2084,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2127,7 +2127,7 @@
         <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D20" s="7">
         <v>2</v>
@@ -2169,38 +2169,38 @@
         <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D23" s="7">
         <v>2</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D24" s="7">
         <v>14</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -2209,44 +2209,44 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D27" s="7">
         <v>1</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="D29" s="7">
         <v>1</v>
@@ -2254,10 +2254,10 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D30" s="7">
         <v>1</v>
@@ -2265,24 +2265,24 @@
     </row>
     <row r="31" spans="1:5" ht="27.6">
       <c r="A31" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D31" s="7">
         <v>1</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D32" s="7">
         <v>2</v>
@@ -2290,13 +2290,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D33" s="7">
         <v>1</v>
@@ -2307,10 +2307,10 @@
         <v>61</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D34" s="7">
         <v>1</v>
@@ -2321,16 +2321,16 @@
         <v>23</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D35" s="7">
         <v>1</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2338,16 +2338,16 @@
         <v>23</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D36" s="7">
         <v>1</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2355,10 +2355,10 @@
         <v>23</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D37" s="7">
         <v>1</v>
@@ -2366,30 +2366,30 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D38" s="7">
         <v>1</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D39" s="7">
         <v>1</v>
@@ -2397,13 +2397,13 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D40" s="7">
         <v>1</v>
@@ -2411,13 +2411,13 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D41" s="7">
         <v>1</v>
@@ -2425,30 +2425,30 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D42" s="7">
         <v>1</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D43" s="7">
         <v>1</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D44" s="7">
         <v>1</v>
@@ -2546,7 +2546,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2554,7 +2554,7 @@
         <v>61</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D53" s="7">
         <v>1</v>
@@ -2566,10 +2566,10 @@
         <v>63</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>218</v>
+        <v>297</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>64</v>
+        <v>296</v>
       </c>
       <c r="D54" s="7">
         <v>1</v>
@@ -2577,38 +2577,38 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D55" s="7">
         <v>1</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="D56" s="7">
         <v>1</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -2617,24 +2617,24 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D59" s="7">
         <v>3</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -2643,38 +2643,38 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D62" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="41.4">
       <c r="A63" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D63" s="7">
         <v>1</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D64" s="7">
         <v>1</v>
@@ -2682,13 +2682,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D65" s="7">
         <v>1</v>
@@ -2696,61 +2696,61 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="27.6">
       <c r="A69" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2770,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6375C457-B0C0-4589-A3C9-93DBFBDBB730}">
   <dimension ref="A2:E47"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="13"/>
@@ -2812,10 +2812,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
@@ -2823,10 +2823,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
@@ -2834,10 +2834,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
@@ -2845,30 +2845,30 @@
     </row>
     <row r="7" spans="1:5" ht="27.6">
       <c r="A7" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
@@ -2876,47 +2876,47 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D9" s="7">
         <v>2</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D11" s="7">
         <v>2</v>
@@ -2924,19 +2924,19 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2944,7 +2944,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="13"/>
@@ -2953,27 +2953,27 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="7">
         <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D16" s="7">
         <v>1</v>
@@ -2981,13 +2981,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
@@ -2995,13 +2995,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D18" s="7">
         <v>12</v>
@@ -3009,13 +3009,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D19" s="7">
         <v>9</v>
@@ -3023,19 +3023,19 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D20" s="7">
         <v>3</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3052,73 +3052,73 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="7">
         <v>50</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
+        <v>299</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>299</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="s">
         <v>126</v>
       </c>
-      <c r="B26" t="s">
-        <v>130</v>
-      </c>
       <c r="C26" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>125</v>
-      </c>
-      <c r="D26" s="7">
-        <v>1</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D27" s="7">
         <v>1</v>
@@ -3127,13 +3127,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D28" s="7">
         <v>12</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D29" s="7">
         <v>9</v>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="13"/>
@@ -3173,13 +3173,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D33" s="7">
         <v>12</v>
@@ -3187,13 +3187,13 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D34" s="7">
         <v>4</v>
@@ -3201,166 +3201,166 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="11" t="s">
+      <c r="D35" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="E35" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>153</v>
+        <v>298</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>269</v>
+        <v>105</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D40" s="7">
+        <v>300</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D41" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="3"/>
-    </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D43" s="7">
-        <v>4</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="A43" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>117</v>
+        <v>76</v>
+      </c>
+      <c r="D44" s="7">
+        <v>4</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>118</v>
-      </c>
       <c r="D45" s="7" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>290</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C46" s="11">
         <v>9225</v>
@@ -3371,13 +3371,13 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D47" s="7">
         <v>1</v>
@@ -3429,7 +3429,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -3438,13 +3438,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D4" s="7">
         <v>2</v>
@@ -3452,13 +3452,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D5" s="7">
         <v>4</v>
@@ -3466,13 +3466,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D6" s="7">
         <v>4</v>
@@ -3480,13 +3480,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D7" s="7">
         <v>5</v>
@@ -3494,13 +3494,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="D8" s="7">
         <v>4</v>
@@ -3508,30 +3508,30 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D9" s="7">
         <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D10" s="7">
         <v>8</v>
@@ -3539,13 +3539,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="D11" s="7">
         <v>2</v>
@@ -3553,13 +3553,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D12" s="7">
         <v>6</v>
@@ -3567,13 +3567,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D13" s="7">
         <v>2</v>
@@ -3581,64 +3581,64 @@
     </row>
     <row r="14" spans="1:5" ht="27.6">
       <c r="A14" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D14" s="7">
         <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D15" s="7">
         <v>4</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D16" s="7">
         <v>4</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D17" s="7">
         <v>4</v>
@@ -3646,13 +3646,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D18" s="7">
         <v>29</v>
@@ -3660,13 +3660,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D19" s="7">
         <v>29</v>
@@ -3674,13 +3674,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D20" s="7">
         <v>8</v>
@@ -3688,13 +3688,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D21" s="7">
         <v>12</v>
@@ -3702,13 +3702,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D22" s="7">
         <v>8</v>
@@ -3716,13 +3716,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D23" s="7">
         <v>4</v>
@@ -3730,13 +3730,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D24" s="7">
         <v>2</v>
@@ -3744,13 +3744,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D25" s="7">
         <v>12</v>
@@ -3758,13 +3758,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D26" s="7">
         <v>10</v>
@@ -3772,13 +3772,13 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D27" s="7">
         <v>8</v>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="6" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -3795,13 +3795,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D30" s="7">
         <v>4</v>
@@ -3809,13 +3809,13 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D31" s="7">
         <v>4</v>
@@ -3823,13 +3823,13 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D32" s="7">
         <v>8</v>
@@ -3837,13 +3837,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D33" s="7">
         <v>18</v>
@@ -3851,7 +3851,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -3860,10 +3860,10 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D36" s="7">
         <v>2</v>
@@ -3871,10 +3871,10 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D37" s="7">
         <v>10</v>
@@ -3882,10 +3882,10 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D38" s="7">
         <v>12</v>
@@ -3893,41 +3893,41 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D39" s="7">
         <v>1</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="13.8" customHeight="1">
       <c r="A40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="D40" s="7">
         <v>32</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D41" s="7">
         <v>8</v>
@@ -3936,30 +3936,30 @@
     </row>
     <row r="42" spans="1:5" ht="13.8" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D42" s="7">
         <v>4</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D43" s="7">
         <v>2</v>
@@ -3968,13 +3968,13 @@
     </row>
     <row r="44" spans="1:5" ht="13.8" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D44" s="7">
         <v>44</v>
@@ -3983,13 +3983,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D45" s="7">
         <v>12</v>
@@ -3998,24 +3998,24 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D46" s="7">
         <v>6</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -4024,19 +4024,19 @@
     </row>
     <row r="49" spans="1:5" ht="27.6">
       <c r="A49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="D49" s="7">
         <v>2</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot 4 Screws, literally unbuildable
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3d printing\stormwalker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF0B3AD-8081-49B8-92FD-FE019DE10D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1491B435-9629-40F9-B3BB-EC819885CD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="27276" windowHeight="22044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="27276" windowHeight="22044" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Body" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="306">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1189,10 +1189,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Lower than 2mm head height, so it can sink below the magnetic sheet.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Magnetic Sheet</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1410,6 +1406,22 @@
   </si>
   <si>
     <t>For making custom RTV silicone socks. Rinse the mold with dish soap water.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self Tapping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M2x10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For X and Y endstops.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lower than 1.2mm head height, so it can sink below the magnetic sheet.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1869,7 +1881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
@@ -2456,10 +2468,10 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="D44" s="7">
         <v>1</v>
@@ -2566,10 +2578,10 @@
         <v>63</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D54" s="7">
         <v>1</v>
@@ -2577,19 +2589,19 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>250</v>
-      </c>
       <c r="D55" s="7">
         <v>1</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2603,7 +2615,7 @@
         <v>1</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2696,16 +2708,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>156</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2750,7 +2762,7 @@
         <v>187</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2803,7 +2815,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="13"/>
@@ -2812,10 +2824,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
@@ -2823,10 +2835,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
@@ -2834,10 +2846,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
@@ -2845,30 +2857,30 @@
     </row>
     <row r="7" spans="1:5" ht="27.6">
       <c r="A7" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>269</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>270</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
@@ -2876,47 +2888,47 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D9" s="7">
         <v>2</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D11" s="7">
         <v>2</v>
@@ -2924,19 +2936,19 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="D12" s="7">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2944,7 +2956,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="13"/>
@@ -2953,7 +2965,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>77</v>
@@ -3070,7 +3082,7 @@
         <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>106</v>
@@ -3084,7 +3096,7 @@
         <v>105</v>
       </c>
       <c r="B25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>111</v>
@@ -3227,7 +3239,7 @@
         <v>111</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>148</v>
@@ -3241,13 +3253,13 @@
         <v>110</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D37" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3258,13 +3270,13 @@
         <v>110</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3275,13 +3287,13 @@
         <v>110</v>
       </c>
       <c r="C39" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>258</v>
-      </c>
       <c r="E39" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3289,24 +3301,24 @@
         <v>105</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>111</v>
       </c>
       <c r="D40" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="D41" s="7">
         <v>4</v>
@@ -3357,10 +3369,10 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="C46" s="11">
         <v>9225</v>
@@ -3371,13 +3383,13 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="11" t="s">
         <v>289</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>290</v>
       </c>
       <c r="D47" s="7">
         <v>1</v>
@@ -3394,10 +3406,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D94751F-96BF-42B2-B88F-498F6EAA5B76}">
-  <dimension ref="A2:E49"/>
+  <dimension ref="A2:E50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3441,13 +3453,16 @@
         <v>223</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>220</v>
+        <v>302</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>224</v>
+        <v>303</v>
       </c>
       <c r="D4" s="7">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3458,10 +3473,10 @@
         <v>220</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D5" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3472,7 +3487,7 @@
         <v>220</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D6" s="7">
         <v>4</v>
@@ -3486,10 +3501,10 @@
         <v>220</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D7" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3500,10 +3515,10 @@
         <v>220</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D8" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3514,13 +3529,10 @@
         <v>220</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D9" s="7">
-        <v>12</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>285</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3531,10 +3543,13 @@
         <v>220</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D10" s="7">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3545,10 +3560,10 @@
         <v>220</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D11" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3559,10 +3574,10 @@
         <v>220</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D12" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3573,44 +3588,41 @@
         <v>220</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D13" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="27.6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="D14" s="7">
         <v>2</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+    </row>
+    <row r="15" spans="1:5" ht="27.6">
       <c r="A15" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D15" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>247</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3618,16 +3630,16 @@
         <v>223</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="D16" s="7">
         <v>4</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>232</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3638,10 +3650,13 @@
         <v>221</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D17" s="7">
         <v>4</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3652,10 +3667,10 @@
         <v>221</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="D18" s="7">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3666,7 +3681,7 @@
         <v>221</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="D19" s="7">
         <v>29</v>
@@ -3680,10 +3695,10 @@
         <v>221</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D20" s="7">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3694,10 +3709,10 @@
         <v>221</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D21" s="7">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3708,10 +3723,10 @@
         <v>221</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D22" s="7">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3722,10 +3737,10 @@
         <v>221</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="D23" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3736,10 +3751,10 @@
         <v>221</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="D24" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3750,10 +3765,10 @@
         <v>221</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D25" s="7">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3764,10 +3779,10 @@
         <v>221</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D26" s="7">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3778,34 +3793,34 @@
         <v>221</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D27" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D28" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="6" t="s">
+    <row r="30" spans="1:5">
+      <c r="A30" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D30" s="7">
-        <v>4</v>
-      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
@@ -3815,7 +3830,7 @@
         <v>216</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D31" s="7">
         <v>4</v>
@@ -3826,13 +3841,13 @@
         <v>223</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D32" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3840,44 +3855,47 @@
         <v>223</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D33" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D34" s="7">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="6" t="s">
+    <row r="36" spans="1:5">
+      <c r="A36" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" s="7">
-        <v>2</v>
-      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" s="7">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3885,103 +3903,99 @@
         <v>78</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D38" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="7">
-        <v>1</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="D40" s="7">
+        <v>1</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="13.8" customHeight="1">
-      <c r="A40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" s="7">
-        <v>32</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" ht="13.8" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="7">
+        <v>32</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D42" s="7">
         <v>8</v>
       </c>
-      <c r="E41" s="15"/>
-    </row>
-    <row r="42" spans="1:5" ht="13.8" customHeight="1">
-      <c r="A42" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D42" s="7">
-        <v>4</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="E42" s="15"/>
+    </row>
+    <row r="43" spans="1:5" ht="13.8" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="D43" s="7">
-        <v>2</v>
-      </c>
-      <c r="E43" s="15"/>
-    </row>
-    <row r="44" spans="1:5" ht="13.8" customHeight="1">
+        <v>4</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>284</v>
+        <v>151</v>
       </c>
       <c r="D44" s="7">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="E44" s="15"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" ht="13.8" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>90</v>
       </c>
@@ -3989,10 +4003,10 @@
         <v>95</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>96</v>
+        <v>283</v>
       </c>
       <c r="D45" s="7">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="E45" s="15"/>
     </row>
@@ -4001,48 +4015,63 @@
         <v>90</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="7">
+        <v>12</v>
+      </c>
+      <c r="E46" s="15"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D47" s="7">
         <v>6</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E47" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="6" t="s">
+    <row r="49" spans="1:5">
+      <c r="A49" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" ht="27.6">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" ht="27.6">
+      <c r="A50" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D50" s="7">
         <v>2</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="E43:E46"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>